<commit_message>
Minor correction with enums, added a new step in geneartion logic
</commit_message>
<xml_diff>
--- a/RoughWork.xlsx
+++ b/RoughWork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\QRGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C08CA-A4CC-4352-874E-3D1F5CFF7A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9FCDE-BF6D-45EC-8656-DAC6DAA3E36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{A44875FE-E1BB-411C-91C2-98D22DF076E8}"/>
   </bookViews>
@@ -30,6 +30,54 @@
     <author>Darshan GA</author>
   </authors>
   <commentList>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{9C3037CC-76CD-4E23-A22B-6DD1F892313D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error Correction level</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{BD856ED2-F684-4CC7-ACF1-510047E346C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error Correction level</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="L25" authorId="0" shapeId="0" xr:uid="{DB395FB7-5443-42FD-8814-D9388AA928B6}">
       <text>
         <r>
@@ -57,12 +105,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="L31" authorId="0" shapeId="0" xr:uid="{38113769-3984-4E35-94B8-0588D342FCCA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error correction level</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L32" authorId="0" shapeId="0" xr:uid="{DEA1FEBB-3CA5-40BC-8F71-7C679C9C0EC3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error correction level</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Alogorithm</t>
   </si>
@@ -81,12 +177,57 @@
   <si>
     <t>Start common index: for</t>
   </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <t>F15</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +248,27 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +290,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,12 +333,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3BB37B-C476-4A05-A272-CDA0D3D0E1A6}">
   <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="72" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,37 +945,59 @@
       <c r="J7" s="3">
         <v>6</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
+      <c r="K7" s="3">
+        <v>7</v>
+      </c>
+      <c r="L7" s="3">
+        <v>8</v>
+      </c>
+      <c r="M7" s="3">
+        <v>9</v>
+      </c>
+      <c r="N7" s="3">
+        <v>10</v>
+      </c>
+      <c r="O7" s="3">
+        <v>11</v>
+      </c>
+      <c r="P7" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>13</v>
+      </c>
+      <c r="R7" s="3">
+        <v>14</v>
+      </c>
+      <c r="S7" s="3">
+        <v>15</v>
+      </c>
+      <c r="T7" s="3">
+        <v>16</v>
+      </c>
+      <c r="U7" s="3">
+        <v>17</v>
+      </c>
       <c r="V7" s="3">
+        <v>18</v>
+      </c>
+      <c r="W7" s="3">
         <v>19</v>
       </c>
-      <c r="W7" s="3">
+      <c r="X7" s="3">
         <v>20</v>
       </c>
-      <c r="X7" s="3">
+      <c r="Y7" s="3">
         <v>21</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="Z7" s="3">
         <v>22</v>
       </c>
-      <c r="Z7" s="3">
+      <c r="AA7" s="3">
         <v>23</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AB7" s="3">
         <v>24</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>25</v>
       </c>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
@@ -823,8 +1019,10 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -833,7 +1031,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="1">
+      <c r="U8" s="6">
         <v>0</v>
       </c>
       <c r="V8" s="2"/>
@@ -863,8 +1061,10 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -873,7 +1073,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="1">
+      <c r="U9" s="6">
         <v>1</v>
       </c>
       <c r="V9" s="2"/>
@@ -903,8 +1103,10 @@
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -913,7 +1115,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
-      <c r="U10" s="1">
+      <c r="U10" s="6">
         <v>2</v>
       </c>
       <c r="V10" s="2"/>
@@ -943,8 +1145,10 @@
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -953,7 +1157,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
-      <c r="U11" s="1">
+      <c r="U11" s="6">
         <v>3</v>
       </c>
       <c r="V11" s="2"/>
@@ -983,8 +1187,10 @@
       <c r="H12" s="2"/>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -993,7 +1199,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="1">
+      <c r="U12" s="6">
         <v>4</v>
       </c>
       <c r="V12" s="2"/>
@@ -1023,8 +1229,10 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1033,7 +1241,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="1">
+      <c r="U13" s="6">
         <v>5</v>
       </c>
       <c r="V13" s="2"/>
@@ -1063,7 +1271,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="1"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="4"/>
       <c r="M14" s="1"/>
       <c r="N14" s="4"/>
@@ -1073,7 +1281,7 @@
       <c r="R14" s="4"/>
       <c r="S14" s="1"/>
       <c r="T14" s="4"/>
-      <c r="U14" s="1">
+      <c r="U14" s="6">
         <v>6</v>
       </c>
       <c r="V14" s="2"/>
@@ -1093,16 +1301,20 @@
         <v>8</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="C15" s="3">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1111,14 +1323,14 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
@@ -1129,16 +1341,34 @@
         <v>9</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="C16" s="3">
+        <v>8</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1147,14 +1377,30 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
+      <c r="U16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
@@ -1165,7 +1411,9 @@
         <v>10</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3">
+        <v>9</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1201,7 +1449,9 @@
         <v>11</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3">
+        <v>10</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1237,7 +1487,9 @@
         <v>12</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3">
+        <v>11</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1273,7 +1525,9 @@
         <v>13</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="3">
+        <v>12</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1309,7 +1563,9 @@
         <v>14</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3">
+        <v>13</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1345,7 +1601,9 @@
         <v>15</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="3">
+        <v>14</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1381,7 +1639,9 @@
         <v>16</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="3">
+        <v>15</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1427,7 +1687,9 @@
         <v>17</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="3">
+        <v>16</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1465,29 +1727,31 @@
         <v>18</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="1">
+      <c r="C25" s="3">
+        <v>17</v>
+      </c>
+      <c r="D25" s="6">
         <v>0</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="6">
         <v>1</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="6">
         <v>2</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="6">
         <v>3</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="6">
         <v>4</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="6">
         <v>5</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="6">
         <v>6</v>
       </c>
-      <c r="K25" s="1"/>
+      <c r="K25" s="6"/>
       <c r="L25" s="4"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1518,7 +1782,7 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1527,8 +1791,10 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1558,7 +1824,7 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
@@ -1567,8 +1833,10 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1598,7 +1866,7 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="1"/>
@@ -1607,8 +1875,10 @@
       <c r="H28" s="2"/>
       <c r="I28" s="1"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -1646,7 +1916,7 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
@@ -1655,8 +1925,10 @@
       <c r="H29" s="2"/>
       <c r="I29" s="1"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -1686,7 +1958,7 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1695,8 +1967,10 @@
       <c r="H30" s="2"/>
       <c r="I30" s="1"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -1726,7 +2000,7 @@
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
@@ -1735,8 +2009,10 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="2"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -1766,7 +2042,7 @@
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1775,8 +2051,10 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -2063,6 +2341,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
logic to add initial format strip pattern and initial data filllogic
</commit_message>
<xml_diff>
--- a/RoughWork.xlsx
+++ b/RoughWork.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\QRGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9FCDE-BF6D-45EC-8656-DAC6DAA3E36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74534410-4B9A-44DC-94A8-1286EB7D1E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{A44875FE-E1BB-411C-91C2-98D22DF076E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A44875FE-E1BB-411C-91C2-98D22DF076E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Position squares" sheetId="1" r:id="rId1"/>
+    <sheet name="SampleRepresentation" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -157,8 +158,141 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Darshan GA</author>
+  </authors>
+  <commentList>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{64A7F13E-9FE5-4919-8B42-AB3D66E033DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error Correction level</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{9D88C406-08C4-4338-8FA0-887864B7F81C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error Correction level</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L25" authorId="0" shapeId="0" xr:uid="{B552ECA4-954B-408F-9A97-0F8156F72F77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Always black by design.
+Row: qrDimension - 7 + 1
+Column: 7 + 1 or 8
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L31" authorId="0" shapeId="0" xr:uid="{01256A3A-ADEC-4767-8F66-028AF184B256}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error correction level</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L32" authorId="0" shapeId="0" xr:uid="{E36B8194-1A3E-4561-937E-45246581CB56}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error correction level</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
   <si>
     <t>Alogorithm</t>
   </si>
@@ -221,6 +355,114 @@
   </si>
   <si>
     <t>F15</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D20</t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>&lt;--- Data start</t>
+  </si>
+  <si>
+    <t>01101000011101000111</t>
+  </si>
+  <si>
+    <t>&lt;---Data Format specifier</t>
+  </si>
+  <si>
+    <t>&lt;-- Data Length specifier</t>
   </si>
 </sst>
 </file>
@@ -268,7 +510,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +547,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -333,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -341,6 +589,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3BB37B-C476-4A05-A272-CDA0D3D0E1A6}">
   <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView showGridLines="0" zoomScale="72" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1437,8 +1687,12 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
+      <c r="AA17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
@@ -1475,8 +1729,12 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
+      <c r="AA18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
@@ -1513,8 +1771,12 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
+      <c r="AA19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
@@ -1551,8 +1813,12 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
+      <c r="AA20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
       <c r="AE20" s="3"/>
@@ -1589,8 +1855,12 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
+      <c r="AA21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
       <c r="AE21" s="3"/>
@@ -1627,8 +1897,12 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
+      <c r="AA22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
       <c r="AE22" s="3"/>
@@ -1675,8 +1949,12 @@
       </c>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
+      <c r="AA23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
       <c r="AE23" s="3"/>
@@ -1715,8 +1993,12 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1"/>
+      <c r="AA24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
@@ -1769,8 +2051,12 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
+      <c r="AA25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
@@ -1811,8 +2097,12 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
-      <c r="AB26" s="1"/>
+      <c r="AA26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB26" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
@@ -1853,8 +2143,12 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
+      <c r="AA27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB27" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
       <c r="AE27" s="3"/>
@@ -1893,17 +2187,13 @@
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
       <c r="X28" s="2"/>
-      <c r="Y28" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z28" s="1">
-        <v>2</v>
-      </c>
-      <c r="AA28" s="1">
-        <v>3</v>
-      </c>
-      <c r="AB28" s="1">
-        <v>4</v>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
@@ -1937,17 +2227,21 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
-      <c r="U29" s="1">
-        <v>1</v>
-      </c>
+      <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="3"/>
+      <c r="AA29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>1</v>
+      </c>
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
@@ -1979,17 +2273,21 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
-      <c r="U30" s="1">
-        <v>2</v>
-      </c>
+      <c r="U30" s="1"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="3"/>
+      <c r="AA30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>2</v>
+      </c>
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
@@ -2021,17 +2319,21 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
-      <c r="U31" s="1">
-        <v>3</v>
-      </c>
+      <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="1"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="3"/>
+      <c r="AA31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>3</v>
+      </c>
       <c r="AD31" s="3"/>
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
@@ -2063,17 +2365,21 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-      <c r="U32" s="1">
-        <v>4</v>
-      </c>
+      <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
-      <c r="AA32" s="1"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="3"/>
+      <c r="AA32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC32" s="3">
+        <v>4</v>
+      </c>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
@@ -2103,10 +2409,18 @@
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
-      <c r="AA33" s="3"/>
-      <c r="AB33" s="3"/>
+      <c r="Y33" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA33" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB33" s="3">
+        <v>4</v>
+      </c>
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
       <c r="AE33" s="3"/>
@@ -2346,4 +2660,1754 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780B5F8F-73FA-4656-90E3-B6FC94EE5FA6}">
+  <dimension ref="A1:AH44"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="34" max="34" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3">
+        <v>7</v>
+      </c>
+      <c r="K4" s="3">
+        <v>8</v>
+      </c>
+      <c r="L4" s="3">
+        <v>9</v>
+      </c>
+      <c r="M4" s="3">
+        <v>10</v>
+      </c>
+      <c r="N4" s="3">
+        <v>11</v>
+      </c>
+      <c r="O4" s="3">
+        <v>12</v>
+      </c>
+      <c r="P4" s="3">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>14</v>
+      </c>
+      <c r="R4" s="3">
+        <v>15</v>
+      </c>
+      <c r="S4" s="3">
+        <v>16</v>
+      </c>
+      <c r="T4" s="3">
+        <v>17</v>
+      </c>
+      <c r="U4" s="3">
+        <v>18</v>
+      </c>
+      <c r="V4" s="3">
+        <v>19</v>
+      </c>
+      <c r="W4" s="3">
+        <v>20</v>
+      </c>
+      <c r="X4" s="3">
+        <v>21</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>22</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>23</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>24</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>25</v>
+      </c>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4</v>
+      </c>
+      <c r="I7" s="3">
+        <v>5</v>
+      </c>
+      <c r="J7" s="3">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3">
+        <v>7</v>
+      </c>
+      <c r="L7" s="3">
+        <v>8</v>
+      </c>
+      <c r="M7" s="3">
+        <v>9</v>
+      </c>
+      <c r="N7" s="3">
+        <v>10</v>
+      </c>
+      <c r="O7" s="3">
+        <v>11</v>
+      </c>
+      <c r="P7" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>13</v>
+      </c>
+      <c r="R7" s="3">
+        <v>14</v>
+      </c>
+      <c r="S7" s="3">
+        <v>15</v>
+      </c>
+      <c r="T7" s="3">
+        <v>16</v>
+      </c>
+      <c r="U7" s="3">
+        <v>17</v>
+      </c>
+      <c r="V7" s="3">
+        <v>18</v>
+      </c>
+      <c r="W7" s="3">
+        <v>19</v>
+      </c>
+      <c r="X7" s="3">
+        <v>20</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>21</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>22</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>23</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>24</v>
+      </c>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="6">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="6">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="6">
+        <v>2</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="6">
+        <v>3</v>
+      </c>
+      <c r="V11" s="2"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="6">
+        <v>4</v>
+      </c>
+      <c r="V12" s="2"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="6">
+        <v>5</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="6">
+        <v>6</v>
+      </c>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
+        <v>8</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AH17" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
+        <v>14</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1</v>
+      </c>
+      <c r="V23" s="1">
+        <v>2</v>
+      </c>
+      <c r="W23" s="1">
+        <v>3</v>
+      </c>
+      <c r="X23" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>17</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
+        <v>17</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6">
+        <v>2</v>
+      </c>
+      <c r="G25" s="6">
+        <v>3</v>
+      </c>
+      <c r="H25" s="6">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6">
+        <v>6</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1">
+        <v>1</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1">
+        <v>2</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
+        <v>19</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1">
+        <v>3</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF27" s="3"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1">
+        <v>4</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF28" s="3"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3">
+        <v>21</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF29" s="3"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3">
+        <v>22</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF30" s="3"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>24</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3">
+        <v>23</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
+        <v>24</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA33" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB33" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="3"/>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="3"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="3"/>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added logic to move pass allignment pattern and minor cleanups
</commit_message>
<xml_diff>
--- a/RoughWork.xlsx
+++ b/RoughWork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\QRGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74534410-4B9A-44DC-94A8-1286EB7D1E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F2C75E-A227-414F-A052-CDB4FFA03507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A44875FE-E1BB-411C-91C2-98D22DF076E8}"/>
   </bookViews>
@@ -2667,7 +2667,7 @@
   <dimension ref="A1:AH44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+      <selection activeCell="T21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added rough work on what is expected
</commit_message>
<xml_diff>
--- a/RoughWork.xlsx
+++ b/RoughWork.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\QRGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F2C75E-A227-414F-A052-CDB4FFA03507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E1EB2C-54BD-4DE2-94C1-BC216829F37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A44875FE-E1BB-411C-91C2-98D22DF076E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A44875FE-E1BB-411C-91C2-98D22DF076E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Position squares" sheetId="1" r:id="rId1"/>
     <sheet name="SampleRepresentation" sheetId="3" r:id="rId2"/>
+    <sheet name="Filling" sheetId="4" r:id="rId3"/>
+    <sheet name="ByteData" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -291,8 +293,141 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Darshan GA</author>
+  </authors>
+  <commentList>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{71BAE7E4-E39C-4F4A-84C0-CE5571CEBDE4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error Correction level</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{518C7746-330A-4D0B-A927-E81E0931B5E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error Correction level</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L25" authorId="0" shapeId="0" xr:uid="{8EB62F78-77D0-49F9-8235-34CBFEDC7438}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Always black by design.
+Row: qrDimension - 7 + 1
+Column: 7 + 1 or 8
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L31" authorId="0" shapeId="0" xr:uid="{E8F9051C-C3DA-4CB8-A284-7DA7A0DA970C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error correction level</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L32" authorId="0" shapeId="0" xr:uid="{618F3821-9709-4C6B-9B4E-15C13974DA36}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darshan GA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Error correction level</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="62">
   <si>
     <t>Alogorithm</t>
   </si>
@@ -464,6 +599,21 @@
   <si>
     <t>&lt;-- Data Length specifier</t>
   </si>
+  <si>
+    <t>ActualDataFirst4Columns</t>
+  </si>
+  <si>
+    <t>3rdColumnPairData</t>
+  </si>
+  <si>
+    <t>4thColumnPairData</t>
+  </si>
+  <si>
+    <t>5thColumnPairData</t>
+  </si>
+  <si>
+    <t>6thColumnPairData</t>
+  </si>
 </sst>
 </file>
 
@@ -581,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -591,6 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,6 +757,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>603827</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1539</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>221673</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>137344</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BA5B5BA-836D-577E-CE53-A1959796D635}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1823027" y="6485466"/>
+          <a:ext cx="8152246" cy="8240714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2666,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780B5F8F-73FA-4656-90E3-B6FC94EE5FA6}">
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="T21" sqref="A21:XFD21"/>
+    <sheetView showGridLines="0" zoomScale="72" workbookViewId="0">
+      <selection activeCell="X29" sqref="A29:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4410,4 +4610,2952 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6112EA7-970C-4567-9046-FFB020775C7A}">
+  <dimension ref="A1:AH39"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="34" max="34" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3">
+        <v>7</v>
+      </c>
+      <c r="K4" s="3">
+        <v>8</v>
+      </c>
+      <c r="L4" s="3">
+        <v>9</v>
+      </c>
+      <c r="M4" s="3">
+        <v>10</v>
+      </c>
+      <c r="N4" s="3">
+        <v>11</v>
+      </c>
+      <c r="O4" s="3">
+        <v>12</v>
+      </c>
+      <c r="P4" s="3">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>14</v>
+      </c>
+      <c r="R4" s="3">
+        <v>15</v>
+      </c>
+      <c r="S4" s="3">
+        <v>16</v>
+      </c>
+      <c r="T4" s="3">
+        <v>17</v>
+      </c>
+      <c r="U4" s="3">
+        <v>18</v>
+      </c>
+      <c r="V4" s="3">
+        <v>19</v>
+      </c>
+      <c r="W4" s="3">
+        <v>20</v>
+      </c>
+      <c r="X4" s="3">
+        <v>21</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>22</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>23</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>24</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>25</v>
+      </c>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4</v>
+      </c>
+      <c r="I7" s="3">
+        <v>5</v>
+      </c>
+      <c r="J7" s="3">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3">
+        <v>7</v>
+      </c>
+      <c r="L7" s="3">
+        <v>8</v>
+      </c>
+      <c r="M7" s="3">
+        <v>9</v>
+      </c>
+      <c r="N7" s="3">
+        <v>10</v>
+      </c>
+      <c r="O7" s="3">
+        <v>11</v>
+      </c>
+      <c r="P7" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>13</v>
+      </c>
+      <c r="R7" s="3">
+        <v>14</v>
+      </c>
+      <c r="S7" s="3">
+        <v>15</v>
+      </c>
+      <c r="T7" s="3">
+        <v>16</v>
+      </c>
+      <c r="U7" s="3">
+        <v>17</v>
+      </c>
+      <c r="V7" s="3">
+        <v>18</v>
+      </c>
+      <c r="W7" s="3">
+        <v>19</v>
+      </c>
+      <c r="X7" s="3">
+        <v>20</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>21</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>22</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>23</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>24</v>
+      </c>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="6">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="6">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="6">
+        <v>2</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="6">
+        <v>3</v>
+      </c>
+      <c r="V11" s="2"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="6">
+        <v>4</v>
+      </c>
+      <c r="V12" s="2"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="6">
+        <v>5</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="6">
+        <v>6</v>
+      </c>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
+        <v>8</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AH17" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
+        <v>14</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1</v>
+      </c>
+      <c r="V23" s="1">
+        <v>2</v>
+      </c>
+      <c r="W23" s="1">
+        <v>3</v>
+      </c>
+      <c r="X23" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>17</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3">
+        <v>17</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6">
+        <v>2</v>
+      </c>
+      <c r="G25" s="6">
+        <v>3</v>
+      </c>
+      <c r="H25" s="6">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6">
+        <v>6</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1">
+        <v>1</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1">
+        <v>2</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
+        <v>19</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1">
+        <v>3</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1">
+        <v>4</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3">
+        <v>21</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3">
+        <v>22</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>24</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3">
+        <v>23</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
+        <v>24</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA33" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB33" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="3"/>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="3"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB4A098-C4DC-4E74-8528-00E7FA6BA848}">
+  <dimension ref="A1:C144"/>
+  <sheetViews>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" s="9">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" s="9">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74" s="9">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75" s="9">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>96</v>
+      </c>
+      <c r="B96" s="9">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>97</v>
+      </c>
+      <c r="B97" s="9">
+        <v>0</v>
+      </c>
+      <c r="C97" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>98</v>
+      </c>
+      <c r="B98" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>100</v>
+      </c>
+      <c r="B100" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>101</v>
+      </c>
+      <c r="B101" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>102</v>
+      </c>
+      <c r="B102" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>103</v>
+      </c>
+      <c r="B103" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>104</v>
+      </c>
+      <c r="B104" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>105</v>
+      </c>
+      <c r="B105" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>106</v>
+      </c>
+      <c r="B106" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>107</v>
+      </c>
+      <c r="B107" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>108</v>
+      </c>
+      <c r="B108" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>109</v>
+      </c>
+      <c r="B109" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>110</v>
+      </c>
+      <c r="B110" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>111</v>
+      </c>
+      <c r="B111" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>112</v>
+      </c>
+      <c r="B112" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>113</v>
+      </c>
+      <c r="B113" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>114</v>
+      </c>
+      <c r="B114" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>115</v>
+      </c>
+      <c r="B115" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>116</v>
+      </c>
+      <c r="B116" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>117</v>
+      </c>
+      <c r="B117" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>118</v>
+      </c>
+      <c r="B118" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>119</v>
+      </c>
+      <c r="B119" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>120</v>
+      </c>
+      <c r="B120" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>121</v>
+      </c>
+      <c r="B121" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>122</v>
+      </c>
+      <c r="B122" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>123</v>
+      </c>
+      <c r="B123" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>124</v>
+      </c>
+      <c r="B124" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>125</v>
+      </c>
+      <c r="B125" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>126</v>
+      </c>
+      <c r="B126" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>127</v>
+      </c>
+      <c r="B127" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>128</v>
+      </c>
+      <c r="B128" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>129</v>
+      </c>
+      <c r="B129" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>130</v>
+      </c>
+      <c r="B130" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>131</v>
+      </c>
+      <c r="B131" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>132</v>
+      </c>
+      <c r="B132" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>133</v>
+      </c>
+      <c r="B133" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>134</v>
+      </c>
+      <c r="B134" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>135</v>
+      </c>
+      <c r="B135" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>136</v>
+      </c>
+      <c r="B136" s="9">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>137</v>
+      </c>
+      <c r="B137" s="9">
+        <v>0</v>
+      </c>
+      <c r="C137" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>138</v>
+      </c>
+      <c r="B138" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>139</v>
+      </c>
+      <c r="B139" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>140</v>
+      </c>
+      <c r="B140" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>141</v>
+      </c>
+      <c r="B141" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>142</v>
+      </c>
+      <c r="B142" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>143</v>
+      </c>
+      <c r="B143" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144" s="9">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>